<commit_message>
Update App QC Info
Update App QC Info
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Anodiam-Info/APP-QC-Info-Details.xlsx
+++ b/Offline/BusinessManagement/Information/Anodiam-Info/APP-QC-Info-Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Anodiam-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F4337-89C6-416C-8896-222D58B11577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E755795-A457-4E1C-98DA-F905E814A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>SlNo</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Closing Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Debasish Nath cannot Login as Sub Admin</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,13 +500,27 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1285491</v>
+      </c>
+      <c r="D3" s="6">
+        <v>45208</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated APP QC details
Updated APP QC details
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Information/Anodiam-Info/APP-QC-Info-Details.xlsx
+++ b/Offline/BusinessManagement/Information/Anodiam-Info/APP-QC-Info-Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Information\Anodiam-Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E755795-A457-4E1C-98DA-F905E814A589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFDCE3B-61C0-4BE8-B35B-0B07919A1983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>SlNo</t>
   </si>
@@ -67,6 +67,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Debasish Nath cannot Login as Sub Admin</t>
+  </si>
+  <si>
+    <t>Cannot Login to App</t>
+  </si>
+  <si>
+    <t>Video Sent</t>
+  </si>
+  <si>
+    <t>Screenshot Sent</t>
   </si>
 </sst>
 </file>
@@ -431,7 +440,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -443,6 +452,7 @@
     <col min="5" max="5" width="19.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -522,18 +532,36 @@
         <v>11</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1285451</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45208</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
+      <c r="I4" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>

</xml_diff>